<commit_message>
Deploying to gh-pages from  @ 2993b6ac7e41be36fae073a0dc088d1f742f9e45 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2021_3-1-2.xlsx
+++ b/assets/excel/2021_3-1-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\GitHub\IM_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE20C1B-EC21-4A11-86F9-2DE5F5BF3C1E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8D658B-13F7-42ED-9EA0-49D47D163E63}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13110" xr2:uid="{28443E91-70EA-4F55-9852-0B3FB8CA690D}"/>
   </bookViews>
@@ -455,6 +455,24 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -484,24 +502,6 @@
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4285,25 +4285,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+    <row r="6" spans="2:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="22"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="14"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="20"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="26"/>
       <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
@@ -4312,28 +4312,28 @@
       </c>
     </row>
     <row r="8" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22" t="s">
+      <c r="B8" s="21"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" spans="2:6" s="23" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="28"/>
+    </row>
+    <row r="9" spans="2:6" s="13" customFormat="1" ht="8.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="24">
+      <c r="C9" s="14">
         <v>1</v>
       </c>
-      <c r="D9" s="24">
+      <c r="D9" s="14">
         <v>2</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="15">
         <v>3</v>
       </c>
-      <c r="F9" s="25">
+      <c r="F9" s="15">
         <v>4</v>
       </c>
     </row>
@@ -4517,21 +4517,21 @@
         <v>18.458086885580258</v>
       </c>
     </row>
-    <row r="20" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B20" s="7">
         <f>[1]B2_neuer_Gebietsstand!A15</f>
         <v>1</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="27">
+      <c r="D20" s="17">
         <v>2020</v>
       </c>
-      <c r="E20" s="28">
+      <c r="E20" s="18">
         <v>26.251010868064462</v>
       </c>
-      <c r="F20" s="28">
+      <c r="F20" s="18">
         <v>15.970729205704254</v>
       </c>
     </row>
@@ -4697,21 +4697,21 @@
         <v>18.585386576040783</v>
       </c>
     </row>
-    <row r="30" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B30" s="7">
         <f>[1]B2_neuer_Gebietsstand!A25</f>
         <v>2</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D30" s="27">
+      <c r="D30" s="17">
         <v>2020</v>
       </c>
-      <c r="E30" s="28">
+      <c r="E30" s="18">
         <v>33.07695612942036</v>
       </c>
-      <c r="F30" s="28">
+      <c r="F30" s="18">
         <v>21.793494607485066</v>
       </c>
     </row>
@@ -4913,21 +4913,21 @@
         <v>11.148086522462561</v>
       </c>
     </row>
-    <row r="42" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B42" s="7">
         <f>[1]B2_neuer_Gebietsstand!A37</f>
         <v>3</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D42" s="27">
+      <c r="D42" s="17">
         <v>2020</v>
       </c>
-      <c r="E42" s="28">
+      <c r="E42" s="18">
         <v>19.415095338048786</v>
       </c>
-      <c r="F42" s="28">
+      <c r="F42" s="18">
         <v>11.537579595364507</v>
       </c>
     </row>
@@ -5237,39 +5237,39 @@
         <v>6.8651275820170108</v>
       </c>
     </row>
-    <row r="60" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B60" s="7">
         <f>[1]B2_neuer_Gebietsstand!A55</f>
         <v>4</v>
       </c>
-      <c r="C60" s="27" t="s">
+      <c r="C60" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D60" s="27">
+      <c r="D60" s="17">
         <v>2020</v>
       </c>
-      <c r="E60" s="28">
+      <c r="E60" s="18">
         <v>22.11221903791952</v>
       </c>
-      <c r="F60" s="28">
+      <c r="F60" s="18">
         <v>14.665687690959475</v>
       </c>
     </row>
-    <row r="61" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B61" s="7">
         <f>[1]B2_neuer_Gebietsstand!A56</f>
         <v>0</v>
       </c>
-      <c r="C61" s="27" t="s">
+      <c r="C61" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D61" s="27">
+      <c r="D61" s="17">
         <v>2020</v>
       </c>
-      <c r="E61" s="28">
+      <c r="E61" s="18">
         <v>25.255586597516562</v>
       </c>
-      <c r="F61" s="28">
+      <c r="F61" s="18">
         <v>16.142753952754223</v>
       </c>
     </row>
@@ -5453,21 +5453,21 @@
         <v>18.602029312288611</v>
       </c>
     </row>
-    <row r="72" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="72" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B72" s="7">
         <f>[1]B2_neuer_Gebietsstand!A67</f>
         <v>1</v>
       </c>
-      <c r="C72" s="27" t="s">
+      <c r="C72" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D72" s="27">
+      <c r="D72" s="17">
         <v>2019</v>
       </c>
-      <c r="E72" s="28">
+      <c r="E72" s="18">
         <v>26.928366298588358</v>
       </c>
-      <c r="F72" s="28">
+      <c r="F72" s="18">
         <v>16.927557335274845</v>
       </c>
     </row>
@@ -5633,21 +5633,21 @@
         <v>19.764397905759161</v>
       </c>
     </row>
-    <row r="82" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="82" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B82" s="7">
         <f>[1]B2_neuer_Gebietsstand!A77</f>
         <v>2</v>
       </c>
-      <c r="C82" s="27" t="s">
+      <c r="C82" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D82" s="27">
+      <c r="D82" s="17">
         <v>2019</v>
       </c>
-      <c r="E82" s="28">
+      <c r="E82" s="18">
         <v>32.814122533748701</v>
       </c>
-      <c r="F82" s="28">
+      <c r="F82" s="18">
         <v>21.645971362964914</v>
       </c>
     </row>
@@ -5849,21 +5849,21 @@
         <v>13.957446808510637</v>
       </c>
     </row>
-    <row r="94" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="94" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B94" s="7">
         <f>[1]B2_neuer_Gebietsstand!A89</f>
         <v>3</v>
       </c>
-      <c r="C94" s="27" t="s">
+      <c r="C94" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D94" s="27">
+      <c r="D94" s="17">
         <v>2019</v>
       </c>
-      <c r="E94" s="28">
+      <c r="E94" s="18">
         <v>19.862466886816417</v>
       </c>
-      <c r="F94" s="28">
+      <c r="F94" s="18">
         <v>11.403636099720579</v>
       </c>
     </row>
@@ -6173,39 +6173,39 @@
         <v>4.709677419354839</v>
       </c>
     </row>
-    <row r="112" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="112" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B112" s="7">
         <f>[1]B2_neuer_Gebietsstand!A107</f>
         <v>4</v>
       </c>
-      <c r="C112" s="27" t="s">
+      <c r="C112" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D112" s="27">
+      <c r="D112" s="17">
         <v>2019</v>
       </c>
-      <c r="E112" s="28">
+      <c r="E112" s="18">
         <v>22.202736748505654</v>
       </c>
-      <c r="F112" s="28">
+      <c r="F112" s="18">
         <v>14.400039519834015</v>
       </c>
     </row>
-    <row r="113" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="113" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B113" s="7">
         <f>[1]B2_neuer_Gebietsstand!A108</f>
         <v>0</v>
       </c>
-      <c r="C113" s="27" t="s">
+      <c r="C113" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D113" s="27">
+      <c r="D113" s="17">
         <v>2019</v>
       </c>
-      <c r="E113" s="28">
+      <c r="E113" s="18">
         <v>25.472519249325536</v>
       </c>
-      <c r="F113" s="28">
+      <c r="F113" s="18">
         <v>16.193064335085957</v>
       </c>
     </row>
@@ -6389,21 +6389,21 @@
         <v>15.576356752208667</v>
       </c>
     </row>
-    <row r="124" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="124" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B124" s="7">
         <f>[1]B2_neuer_Gebietsstand!A119</f>
         <v>1</v>
       </c>
-      <c r="C124" s="27" t="s">
+      <c r="C124" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D124" s="27">
+      <c r="D124" s="17">
         <v>2018</v>
       </c>
-      <c r="E124" s="28">
+      <c r="E124" s="18">
         <v>24.965085982282439</v>
       </c>
-      <c r="F124" s="28">
+      <c r="F124" s="18">
         <v>14.774361646690984</v>
       </c>
     </row>
@@ -6569,21 +6569,21 @@
         <v>15.226432532347506</v>
       </c>
     </row>
-    <row r="134" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="134" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B134" s="7">
         <f>[1]B2_neuer_Gebietsstand!A129</f>
         <v>2</v>
       </c>
-      <c r="C134" s="27" t="s">
+      <c r="C134" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D134" s="27">
+      <c r="D134" s="17">
         <v>2018</v>
       </c>
-      <c r="E134" s="28">
+      <c r="E134" s="18">
         <v>30.94131275292985</v>
       </c>
-      <c r="F134" s="28">
+      <c r="F134" s="18">
         <v>19.310676836515171</v>
       </c>
     </row>
@@ -6785,21 +6785,21 @@
         <v>13.439930855661192</v>
       </c>
     </row>
-    <row r="146" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="146" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B146" s="7">
         <f>[1]B2_neuer_Gebietsstand!A141</f>
         <v>3</v>
       </c>
-      <c r="C146" s="27" t="s">
+      <c r="C146" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D146" s="27">
+      <c r="D146" s="17">
         <v>2018</v>
       </c>
-      <c r="E146" s="28">
+      <c r="E146" s="18">
         <v>19.130223245195456</v>
       </c>
-      <c r="F146" s="28">
+      <c r="F146" s="18">
         <v>10.546604539755609</v>
       </c>
     </row>
@@ -7109,39 +7109,39 @@
         <v>5.1013734466971874</v>
       </c>
     </row>
-    <row r="164" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="164" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B164" s="7">
         <f>[1]B2_neuer_Gebietsstand!A159</f>
         <v>4</v>
       </c>
-      <c r="C164" s="27" t="s">
+      <c r="C164" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D164" s="27">
+      <c r="D164" s="17">
         <v>2018</v>
       </c>
-      <c r="E164" s="28">
+      <c r="E164" s="18">
         <v>21.340061892471461</v>
       </c>
-      <c r="F164" s="28">
+      <c r="F164" s="18">
         <v>13.306881364202525</v>
       </c>
     </row>
-    <row r="165" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="165" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B165" s="7">
         <f>[1]B2_neuer_Gebietsstand!A160</f>
         <v>0</v>
       </c>
-      <c r="C165" s="27" t="s">
+      <c r="C165" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D165" s="27">
+      <c r="D165" s="17">
         <v>2018</v>
       </c>
-      <c r="E165" s="28">
+      <c r="E165" s="18">
         <v>24.164028613048398</v>
       </c>
-      <c r="F165" s="28">
+      <c r="F165" s="18">
         <v>14.616987166445586</v>
       </c>
     </row>
@@ -7325,21 +7325,21 @@
         <v>14.86341148634115</v>
       </c>
     </row>
-    <row r="176" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="176" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B176" s="7">
         <f>[1]B2_neuer_Gebietsstand!A171</f>
         <v>1</v>
       </c>
-      <c r="C176" s="27" t="s">
+      <c r="C176" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D176" s="27">
+      <c r="D176" s="17">
         <v>2017</v>
       </c>
-      <c r="E176" s="28">
+      <c r="E176" s="18">
         <v>24.182086059713136</v>
       </c>
-      <c r="F176" s="28">
+      <c r="F176" s="18">
         <v>14.232785890713698</v>
       </c>
     </row>
@@ -7505,21 +7505,21 @@
         <v>14.326923076923077</v>
       </c>
     </row>
-    <row r="186" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="186" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B186" s="7">
         <f>[1]B2_neuer_Gebietsstand!A181</f>
         <v>2</v>
       </c>
-      <c r="C186" s="27" t="s">
+      <c r="C186" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D186" s="27">
+      <c r="D186" s="17">
         <v>2017</v>
       </c>
-      <c r="E186" s="28">
+      <c r="E186" s="18">
         <v>29.89403581931629</v>
       </c>
-      <c r="F186" s="28">
+      <c r="F186" s="18">
         <v>18.570961768870493</v>
       </c>
     </row>
@@ -7721,21 +7721,21 @@
         <v>12.259559675550404</v>
       </c>
     </row>
-    <row r="198" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="198" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B198" s="7">
         <f>[1]B2_neuer_Gebietsstand!A193</f>
         <v>3</v>
       </c>
-      <c r="C198" s="27" t="s">
+      <c r="C198" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D198" s="27">
+      <c r="D198" s="17">
         <v>2017</v>
       </c>
-      <c r="E198" s="28">
+      <c r="E198" s="18">
         <v>18.010151494525584</v>
       </c>
-      <c r="F198" s="28">
+      <c r="F198" s="18">
         <v>10.314851908753234</v>
       </c>
     </row>
@@ -8045,39 +8045,39 @@
         <v>6.7020570670205712</v>
       </c>
     </row>
-    <row r="216" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="216" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B216" s="7">
         <f>[1]B2_neuer_Gebietsstand!A211</f>
         <v>4</v>
       </c>
-      <c r="C216" s="27" t="s">
+      <c r="C216" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D216" s="27">
+      <c r="D216" s="17">
         <v>2017</v>
       </c>
-      <c r="E216" s="28">
+      <c r="E216" s="18">
         <v>21.426120013727925</v>
       </c>
-      <c r="F216" s="28">
+      <c r="F216" s="18">
         <v>12.370970722563953</v>
       </c>
     </row>
-    <row r="217" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="217" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B217" s="7">
         <f>[1]B2_neuer_Gebietsstand!A212</f>
         <v>0</v>
       </c>
-      <c r="C217" s="27" t="s">
+      <c r="C217" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D217" s="27">
+      <c r="D217" s="17">
         <v>2017</v>
       </c>
-      <c r="E217" s="28">
+      <c r="E217" s="18">
         <v>23.512626262626263</v>
       </c>
-      <c r="F217" s="28">
+      <c r="F217" s="18">
         <v>13.964646464646465</v>
       </c>
     </row>
@@ -8261,21 +8261,21 @@
         <v>13.783665425881322</v>
       </c>
     </row>
-    <row r="228" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="228" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B228" s="7">
         <f>[1]B2_neuer_Gebietsstand!A223</f>
         <v>1</v>
       </c>
-      <c r="C228" s="27" t="s">
+      <c r="C228" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D228" s="27">
+      <c r="D228" s="17">
         <v>2016</v>
       </c>
-      <c r="E228" s="28">
+      <c r="E228" s="18">
         <v>23.553159867793529</v>
       </c>
-      <c r="F228" s="28">
+      <c r="F228" s="18">
         <v>13.249484261662342</v>
       </c>
     </row>
@@ -8441,21 +8441,21 @@
         <v>11.35295572594608</v>
       </c>
     </row>
-    <row r="238" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="238" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B238" s="7">
         <f>[1]B2_neuer_Gebietsstand!A233</f>
         <v>2</v>
       </c>
-      <c r="C238" s="27" t="s">
+      <c r="C238" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D238" s="27">
+      <c r="D238" s="17">
         <v>2016</v>
       </c>
-      <c r="E238" s="28">
+      <c r="E238" s="18">
         <v>29.497828361284594</v>
       </c>
-      <c r="F238" s="28">
+      <c r="F238" s="18">
         <v>17.518942396094221</v>
       </c>
     </row>
@@ -8657,21 +8657,21 @@
         <v>11.215629522431259</v>
       </c>
     </row>
-    <row r="250" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="250" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B250" s="7">
         <f>[1]B2_neuer_Gebietsstand!A245</f>
         <v>3</v>
       </c>
-      <c r="C250" s="27" t="s">
+      <c r="C250" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D250" s="27">
+      <c r="D250" s="17">
         <v>2016</v>
       </c>
-      <c r="E250" s="28">
+      <c r="E250" s="18">
         <v>16.947115384615387</v>
       </c>
-      <c r="F250" s="28">
+      <c r="F250" s="18">
         <v>8.7119391025641022</v>
       </c>
     </row>
@@ -8981,39 +8981,39 @@
         <v>6.6330209084354719</v>
       </c>
     </row>
-    <row r="268" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="268" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B268" s="7">
         <f>[1]B2_neuer_Gebietsstand!A263</f>
         <v>4</v>
       </c>
-      <c r="C268" s="27" t="s">
+      <c r="C268" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D268" s="27">
+      <c r="D268" s="17">
         <v>2016</v>
       </c>
-      <c r="E268" s="28">
+      <c r="E268" s="18">
         <v>20.621283126421659</v>
       </c>
-      <c r="F268" s="28">
+      <c r="F268" s="18">
         <v>11.203376359998904</v>
       </c>
     </row>
-    <row r="269" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="269" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B269" s="7">
         <f>[1]B2_neuer_Gebietsstand!A264</f>
         <v>0</v>
       </c>
-      <c r="C269" s="27" t="s">
+      <c r="C269" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D269" s="27">
+      <c r="D269" s="17">
         <v>2016</v>
       </c>
-      <c r="E269" s="28">
+      <c r="E269" s="18">
         <v>22.823015168891871</v>
       </c>
-      <c r="F269" s="28">
+      <c r="F269" s="18">
         <v>12.788609265791012</v>
       </c>
     </row>
@@ -9197,21 +9197,21 @@
         <v>12.799643215520126</v>
       </c>
     </row>
-    <row r="280" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="280" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B280" s="7">
         <f>[1]B2_neuer_Gebietsstand!A275</f>
         <v>1</v>
       </c>
-      <c r="C280" s="27" t="s">
+      <c r="C280" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D280" s="27">
+      <c r="D280" s="17">
         <v>2015</v>
       </c>
-      <c r="E280" s="28">
+      <c r="E280" s="18">
         <v>23.338831025055917</v>
       </c>
-      <c r="F280" s="28">
+      <c r="F280" s="18">
         <v>12.344953796796275</v>
       </c>
     </row>
@@ -9377,21 +9377,21 @@
         <v>11.26401630988787</v>
       </c>
     </row>
-    <row r="290" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="290" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B290" s="7">
         <f>[1]B2_neuer_Gebietsstand!A285</f>
         <v>2</v>
       </c>
-      <c r="C290" s="27" t="s">
+      <c r="C290" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D290" s="27">
+      <c r="D290" s="17">
         <v>2015</v>
       </c>
-      <c r="E290" s="28">
+      <c r="E290" s="18">
         <v>28.753400335554069</v>
       </c>
-      <c r="F290" s="28">
+      <c r="F290" s="18">
         <v>16.526852470231791</v>
       </c>
     </row>
@@ -9593,21 +9593,21 @@
         <v>9.282178217821782</v>
       </c>
     </row>
-    <row r="302" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="302" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B302" s="7">
         <f>[1]B2_neuer_Gebietsstand!A297</f>
         <v>3</v>
       </c>
-      <c r="C302" s="27" t="s">
+      <c r="C302" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D302" s="27">
+      <c r="D302" s="17">
         <v>2015</v>
       </c>
-      <c r="E302" s="28">
+      <c r="E302" s="18">
         <v>15.879219911298325</v>
       </c>
-      <c r="F302" s="28">
+      <c r="F302" s="18">
         <v>7.4505356528078739</v>
       </c>
     </row>
@@ -9917,39 +9917,39 @@
         <v>7.0403280929596717</v>
       </c>
     </row>
-    <row r="320" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="320" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B320" s="7">
         <f>[1]B2_neuer_Gebietsstand!A315</f>
         <v>4</v>
       </c>
-      <c r="C320" s="27" t="s">
+      <c r="C320" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D320" s="27">
+      <c r="D320" s="17">
         <v>2015</v>
       </c>
-      <c r="E320" s="28">
+      <c r="E320" s="18">
         <v>19.4612363150124</v>
       </c>
-      <c r="F320" s="28">
+      <c r="F320" s="18">
         <v>10.091372538095106</v>
       </c>
     </row>
-    <row r="321" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="321" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B321" s="7">
         <f>[1]B2_neuer_Gebietsstand!A316</f>
         <v>0</v>
       </c>
-      <c r="C321" s="27" t="s">
+      <c r="C321" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D321" s="27">
+      <c r="D321" s="17">
         <v>2015</v>
       </c>
-      <c r="E321" s="28">
+      <c r="E321" s="18">
         <v>21.953047503582056</v>
       </c>
-      <c r="F321" s="28">
+      <c r="F321" s="18">
         <v>11.698005069987875</v>
       </c>
     </row>
@@ -10133,21 +10133,21 @@
         <v>12.663462613166423</v>
       </c>
     </row>
-    <row r="332" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="332" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B332" s="7">
         <f>[1]B2_neuer_Gebietsstand!A327</f>
         <v>1</v>
       </c>
-      <c r="C332" s="27" t="s">
+      <c r="C332" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D332" s="27">
+      <c r="D332" s="17">
         <v>2014</v>
       </c>
-      <c r="E332" s="28">
+      <c r="E332" s="18">
         <v>22.586487539833559</v>
       </c>
-      <c r="F332" s="28">
+      <c r="F332" s="18">
         <v>12.336367179440153</v>
       </c>
     </row>
@@ -10313,21 +10313,21 @@
         <v>9.0233273519610364</v>
       </c>
     </row>
-    <row r="342" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="342" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B342" s="7">
         <f>[1]B2_neuer_Gebietsstand!A337</f>
         <v>2</v>
       </c>
-      <c r="C342" s="27" t="s">
+      <c r="C342" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D342" s="27">
+      <c r="D342" s="17">
         <v>2014</v>
       </c>
-      <c r="E342" s="28">
+      <c r="E342" s="18">
         <v>28.816050198150595</v>
       </c>
-      <c r="F342" s="28">
+      <c r="F342" s="18">
         <v>15.883421400264201</v>
       </c>
     </row>
@@ -10529,21 +10529,21 @@
         <v>9.004263857536996</v>
       </c>
     </row>
-    <row r="354" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="354" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B354" s="7">
         <f>[1]B2_neuer_Gebietsstand!A349</f>
         <v>3</v>
       </c>
-      <c r="C354" s="27" t="s">
+      <c r="C354" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D354" s="27">
+      <c r="D354" s="17">
         <v>2014</v>
       </c>
-      <c r="E354" s="28">
+      <c r="E354" s="18">
         <v>16.055842855098827</v>
       </c>
-      <c r="F354" s="28">
+      <c r="F354" s="18">
         <v>7.6385340228522374</v>
       </c>
     </row>
@@ -10853,39 +10853,39 @@
         <v>6.6844919786096257</v>
       </c>
     </row>
-    <row r="372" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="372" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B372" s="7">
         <f>[1]B2_neuer_Gebietsstand!A367</f>
         <v>4</v>
       </c>
-      <c r="C372" s="27" t="s">
+      <c r="C372" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D372" s="27">
+      <c r="D372" s="17">
         <v>2014</v>
       </c>
-      <c r="E372" s="28">
+      <c r="E372" s="18">
         <v>19.945894155441582</v>
       </c>
-      <c r="F372" s="28">
+      <c r="F372" s="18">
         <v>10.001127205094967</v>
       </c>
     </row>
-    <row r="373" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="373" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B373" s="7">
         <f>[1]B2_neuer_Gebietsstand!A368</f>
         <v>0</v>
       </c>
-      <c r="C373" s="27" t="s">
+      <c r="C373" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D373" s="27">
+      <c r="D373" s="17">
         <v>2014</v>
       </c>
-      <c r="E373" s="28">
+      <c r="E373" s="18">
         <v>22.007908101787802</v>
       </c>
-      <c r="F373" s="28">
+      <c r="F373" s="18">
         <v>11.529673232949829</v>
       </c>
     </row>
@@ -11069,21 +11069,21 @@
         <v>12.076435951560939</v>
       </c>
     </row>
-    <row r="384" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="384" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B384" s="7">
         <f>[1]B2_neuer_Gebietsstand!A379</f>
         <v>1</v>
       </c>
-      <c r="C384" s="27" t="s">
+      <c r="C384" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D384" s="27">
+      <c r="D384" s="17">
         <v>2013</v>
       </c>
-      <c r="E384" s="28">
+      <c r="E384" s="18">
         <v>22.168495443555887</v>
       </c>
-      <c r="F384" s="28">
+      <c r="F384" s="18">
         <v>11.979263529849359</v>
       </c>
     </row>
@@ -11249,21 +11249,21 @@
         <v>8.3418628454452399</v>
       </c>
     </row>
-    <row r="394" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="394" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B394" s="7">
         <f>[1]B2_neuer_Gebietsstand!A389</f>
         <v>2</v>
       </c>
-      <c r="C394" s="27" t="s">
+      <c r="C394" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D394" s="27">
+      <c r="D394" s="17">
         <v>2013</v>
       </c>
-      <c r="E394" s="28">
+      <c r="E394" s="18">
         <v>28.857385398981322</v>
       </c>
-      <c r="F394" s="28">
+      <c r="F394" s="18">
         <v>15.568760611205432</v>
       </c>
     </row>
@@ -11465,21 +11465,21 @@
         <v>10.526315789473683</v>
       </c>
     </row>
-    <row r="406" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="406" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B406" s="7">
         <f>[1]B2_neuer_Gebietsstand!A401</f>
         <v>3</v>
       </c>
-      <c r="C406" s="27" t="s">
+      <c r="C406" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D406" s="27">
+      <c r="D406" s="17">
         <v>2013</v>
       </c>
-      <c r="E406" s="28">
+      <c r="E406" s="18">
         <v>15.669771521657408</v>
       </c>
-      <c r="F406" s="28">
+      <c r="F406" s="18">
         <v>7.3096361889645385</v>
       </c>
     </row>
@@ -11789,39 +11789,39 @@
         <v>2.3672883787661405</v>
       </c>
     </row>
-    <row r="424" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="424" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B424" s="7">
         <f>[1]B2_neuer_Gebietsstand!A419</f>
         <v>4</v>
       </c>
-      <c r="C424" s="27" t="s">
+      <c r="C424" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D424" s="27">
+      <c r="D424" s="17">
         <v>2013</v>
       </c>
-      <c r="E424" s="28">
+      <c r="E424" s="18">
         <v>21.170205109751709</v>
       </c>
-      <c r="F424" s="28">
+      <c r="F424" s="18">
         <v>10.708888089240734</v>
       </c>
     </row>
-    <row r="425" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="425" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B425" s="7">
         <f>[1]B2_neuer_Gebietsstand!A420</f>
         <v>0</v>
       </c>
-      <c r="C425" s="27" t="s">
+      <c r="C425" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D425" s="27">
+      <c r="D425" s="17">
         <v>2013</v>
       </c>
-      <c r="E425" s="28">
+      <c r="E425" s="18">
         <v>22.229823097234956</v>
       </c>
-      <c r="F425" s="28">
+      <c r="F425" s="18">
         <v>11.5212543267981</v>
       </c>
     </row>
@@ -12005,21 +12005,21 @@
         <v>13.312345401394198</v>
       </c>
     </row>
-    <row r="436" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="436" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B436" s="7">
         <f>[1]B2_neuer_Gebietsstand!A431</f>
         <v>1</v>
       </c>
-      <c r="C436" s="27" t="s">
+      <c r="C436" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D436" s="27">
+      <c r="D436" s="17">
         <v>2012</v>
       </c>
-      <c r="E436" s="28">
+      <c r="E436" s="18">
         <v>22.785912707754601</v>
       </c>
-      <c r="F436" s="28">
+      <c r="F436" s="18">
         <v>12.411130467536138</v>
       </c>
     </row>
@@ -12185,21 +12185,21 @@
         <v>8.6658195679796695</v>
       </c>
     </row>
-    <row r="446" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="446" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B446" s="7">
         <f>[1]B2_neuer_Gebietsstand!A441</f>
         <v>2</v>
       </c>
-      <c r="C446" s="27" t="s">
+      <c r="C446" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D446" s="27">
+      <c r="D446" s="17">
         <v>2012</v>
       </c>
-      <c r="E446" s="28">
+      <c r="E446" s="18">
         <v>28.619213504566805</v>
       </c>
-      <c r="F446" s="28">
+      <c r="F446" s="18">
         <v>15.539264112029672</v>
       </c>
     </row>
@@ -12401,21 +12401,21 @@
         <v>11.947019867549669</v>
       </c>
     </row>
-    <row r="458" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="458" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B458" s="7">
         <f>[1]B2_neuer_Gebietsstand!A453</f>
         <v>3</v>
       </c>
-      <c r="C458" s="27" t="s">
+      <c r="C458" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D458" s="27">
+      <c r="D458" s="17">
         <v>2012</v>
       </c>
-      <c r="E458" s="28">
+      <c r="E458" s="18">
         <v>16.398146573711951</v>
       </c>
-      <c r="F458" s="28">
+      <c r="F458" s="18">
         <v>7.6602618602278527</v>
       </c>
     </row>
@@ -12725,39 +12725,39 @@
         <v>6.1527057079318013</v>
       </c>
     </row>
-    <row r="476" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="476" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B476" s="7">
         <f>[1]B2_neuer_Gebietsstand!A471</f>
         <v>4</v>
       </c>
-      <c r="C476" s="27" t="s">
+      <c r="C476" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D476" s="27">
+      <c r="D476" s="17">
         <v>2012</v>
       </c>
-      <c r="E476" s="28">
+      <c r="E476" s="18">
         <v>22.23138548539114</v>
       </c>
-      <c r="F476" s="28">
+      <c r="F476" s="18">
         <v>11.58105560791706</v>
       </c>
     </row>
-    <row r="477" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="477" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B477" s="7">
         <f>[1]B2_neuer_Gebietsstand!A472</f>
         <v>0</v>
       </c>
-      <c r="C477" s="27" t="s">
+      <c r="C477" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D477" s="27">
+      <c r="D477" s="17">
         <v>2012</v>
       </c>
-      <c r="E477" s="28">
+      <c r="E477" s="18">
         <v>22.778425967675208</v>
       </c>
-      <c r="F477" s="28">
+      <c r="F477" s="18">
         <v>11.949109604005038</v>
       </c>
     </row>
@@ -12941,21 +12941,21 @@
         <v>11.258049678012879</v>
       </c>
     </row>
-    <row r="488" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="488" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B488" s="7">
         <f>[1]B2_neuer_Gebietsstand!A483</f>
         <v>1</v>
       </c>
-      <c r="C488" s="27" t="s">
+      <c r="C488" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D488" s="27">
+      <c r="D488" s="17">
         <v>2011</v>
       </c>
-      <c r="E488" s="28">
+      <c r="E488" s="18">
         <v>21.113649620843866</v>
       </c>
-      <c r="F488" s="28">
+      <c r="F488" s="18">
         <v>11.058720591094692</v>
       </c>
     </row>
@@ -13121,21 +13121,21 @@
         <v>8.6497359818959012</v>
       </c>
     </row>
-    <row r="498" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="498" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B498" s="7">
         <f>[1]B2_neuer_Gebietsstand!A493</f>
         <v>2</v>
       </c>
-      <c r="C498" s="27" t="s">
+      <c r="C498" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D498" s="27">
+      <c r="D498" s="17">
         <v>2011</v>
       </c>
-      <c r="E498" s="28">
+      <c r="E498" s="18">
         <v>27.054126651212425</v>
       </c>
-      <c r="F498" s="28">
+      <c r="F498" s="18">
         <v>15.99514295176068</v>
       </c>
     </row>
@@ -13337,21 +13337,21 @@
         <v>11.046990931574609</v>
       </c>
     </row>
-    <row r="510" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="510" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B510" s="7">
         <f>[1]B2_neuer_Gebietsstand!A505</f>
         <v>3</v>
       </c>
-      <c r="C510" s="27" t="s">
+      <c r="C510" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D510" s="27">
+      <c r="D510" s="17">
         <v>2011</v>
       </c>
-      <c r="E510" s="28">
+      <c r="E510" s="18">
         <v>16.681738976994509</v>
       </c>
-      <c r="F510" s="28">
+      <c r="F510" s="18">
         <v>8.2427156627037519</v>
       </c>
     </row>
@@ -13661,39 +13661,39 @@
         <v>5.5891238670694863</v>
       </c>
     </row>
-    <row r="528" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="528" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B528" s="7">
         <f>[1]B2_neuer_Gebietsstand!A523</f>
         <v>4</v>
       </c>
-      <c r="C528" s="27" t="s">
+      <c r="C528" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D528" s="27">
+      <c r="D528" s="17">
         <v>2011</v>
       </c>
-      <c r="E528" s="28">
+      <c r="E528" s="18">
         <v>21.563014605167982</v>
       </c>
-      <c r="F528" s="28">
+      <c r="F528" s="18">
         <v>11.294765840220386</v>
       </c>
     </row>
-    <row r="529" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="529" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B529" s="7">
         <f>[1]B2_neuer_Gebietsstand!A524</f>
         <v>0</v>
       </c>
-      <c r="C529" s="27" t="s">
+      <c r="C529" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D529" s="27">
+      <c r="D529" s="17">
         <v>2011</v>
       </c>
-      <c r="E529" s="28">
+      <c r="E529" s="18">
         <v>21.848094377392961</v>
       </c>
-      <c r="F529" s="28">
+      <c r="F529" s="18">
         <v>11.816609332789147</v>
       </c>
     </row>
@@ -13877,21 +13877,21 @@
         <v>11.258049678012879</v>
       </c>
     </row>
-    <row r="540" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="540" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B540" s="7">
         <f>[1]B2_neuer_Gebietsstand!A535</f>
         <v>1</v>
       </c>
-      <c r="C540" s="27" t="s">
+      <c r="C540" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D540" s="27">
+      <c r="D540" s="17">
         <v>2010</v>
       </c>
-      <c r="E540" s="28">
+      <c r="E540" s="18">
         <v>21.113649620843866</v>
       </c>
-      <c r="F540" s="28">
+      <c r="F540" s="18">
         <v>11.058720591094692</v>
       </c>
     </row>
@@ -14057,21 +14057,21 @@
         <v>8.6497359818959012</v>
       </c>
     </row>
-    <row r="550" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="550" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B550" s="7">
         <f>[1]B2_neuer_Gebietsstand!A545</f>
         <v>2</v>
       </c>
-      <c r="C550" s="27" t="s">
+      <c r="C550" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D550" s="27">
+      <c r="D550" s="17">
         <v>2010</v>
       </c>
-      <c r="E550" s="28">
+      <c r="E550" s="18">
         <v>27.054126651212425</v>
       </c>
-      <c r="F550" s="28">
+      <c r="F550" s="18">
         <v>15.99514295176068</v>
       </c>
     </row>
@@ -14273,21 +14273,21 @@
         <v>11.046990931574609</v>
       </c>
     </row>
-    <row r="562" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="562" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B562" s="7">
         <f>[1]B2_neuer_Gebietsstand!A557</f>
         <v>3</v>
       </c>
-      <c r="C562" s="27" t="s">
+      <c r="C562" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D562" s="27">
+      <c r="D562" s="17">
         <v>2010</v>
       </c>
-      <c r="E562" s="28">
+      <c r="E562" s="18">
         <v>16.681738976994509</v>
       </c>
-      <c r="F562" s="28">
+      <c r="F562" s="18">
         <v>8.2427156627037519</v>
       </c>
     </row>
@@ -14597,39 +14597,39 @@
         <v>5.5891238670694863</v>
       </c>
     </row>
-    <row r="580" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="580" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B580" s="7">
         <f>[1]B2_neuer_Gebietsstand!A575</f>
         <v>4</v>
       </c>
-      <c r="C580" s="27" t="s">
+      <c r="C580" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D580" s="27">
+      <c r="D580" s="17">
         <v>2010</v>
       </c>
-      <c r="E580" s="28">
+      <c r="E580" s="18">
         <v>21.563014605167982</v>
       </c>
-      <c r="F580" s="28">
+      <c r="F580" s="18">
         <v>11.294765840220386</v>
       </c>
     </row>
-    <row r="581" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="581" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B581" s="7">
         <f>[1]B2_neuer_Gebietsstand!A576</f>
         <v>0</v>
       </c>
-      <c r="C581" s="27" t="s">
+      <c r="C581" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D581" s="27">
+      <c r="D581" s="17">
         <v>2010</v>
       </c>
-      <c r="E581" s="28">
+      <c r="E581" s="18">
         <v>21.848094377392961</v>
       </c>
-      <c r="F581" s="28">
+      <c r="F581" s="18">
         <v>11.816609332789147</v>
       </c>
     </row>
@@ -14813,21 +14813,21 @@
         <v>11.386657352427523</v>
       </c>
     </row>
-    <row r="592" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="592" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B592" s="7">
         <f>[1]B2_neuer_Gebietsstand!A587</f>
         <v>1</v>
       </c>
-      <c r="C592" s="27" t="s">
+      <c r="C592" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D592" s="27">
+      <c r="D592" s="17">
         <v>2009</v>
       </c>
-      <c r="E592" s="28">
+      <c r="E592" s="18">
         <v>21.210383263097523</v>
       </c>
-      <c r="F592" s="28">
+      <c r="F592" s="18">
         <v>11.54776450639603</v>
       </c>
     </row>
@@ -14993,21 +14993,21 @@
         <v>7.9001544004117337</v>
       </c>
     </row>
-    <row r="602" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="602" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B602" s="7">
         <f>[1]B2_neuer_Gebietsstand!A597</f>
         <v>2</v>
       </c>
-      <c r="C602" s="27" t="s">
+      <c r="C602" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D602" s="27">
+      <c r="D602" s="17">
         <v>2009</v>
       </c>
-      <c r="E602" s="28">
+      <c r="E602" s="18">
         <v>26.260177646188009</v>
       </c>
-      <c r="F602" s="28">
+      <c r="F602" s="18">
         <v>15.027757216876388</v>
       </c>
     </row>
@@ -15209,21 +15209,21 @@
         <v>10.185690879300928</v>
       </c>
     </row>
-    <row r="614" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="614" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B614" s="7">
         <f>[1]B2_neuer_Gebietsstand!A609</f>
         <v>3</v>
       </c>
-      <c r="C614" s="27" t="s">
+      <c r="C614" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D614" s="27">
+      <c r="D614" s="17">
         <v>2009</v>
       </c>
-      <c r="E614" s="28">
+      <c r="E614" s="18">
         <v>16.308578717040881</v>
       </c>
-      <c r="F614" s="28">
+      <c r="F614" s="18">
         <v>8.0685241791832514</v>
       </c>
     </row>
@@ -15533,39 +15533,39 @@
         <v>7.0411985018726586</v>
       </c>
     </row>
-    <row r="632" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="632" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B632" s="7">
         <f>[1]B2_neuer_Gebietsstand!A627</f>
         <v>4</v>
       </c>
-      <c r="C632" s="27" t="s">
+      <c r="C632" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D632" s="27">
+      <c r="D632" s="17">
         <v>2009</v>
       </c>
-      <c r="E632" s="28">
+      <c r="E632" s="18">
         <v>20.494231368880573</v>
       </c>
-      <c r="F632" s="28">
+      <c r="F632" s="18">
         <v>10.637667602120361</v>
       </c>
     </row>
-    <row r="633" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="633" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B633" s="7">
         <f>[1]B2_neuer_Gebietsstand!A628</f>
         <v>0</v>
       </c>
-      <c r="C633" s="27" t="s">
+      <c r="C633" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D633" s="27">
+      <c r="D633" s="17">
         <v>2009</v>
       </c>
-      <c r="E633" s="28">
+      <c r="E633" s="18">
         <v>21.230295058795814</v>
       </c>
-      <c r="F633" s="28">
+      <c r="F633" s="18">
         <v>11.407762225406859</v>
       </c>
     </row>
@@ -15749,21 +15749,21 @@
         <v>10.653724710560168</v>
       </c>
     </row>
-    <row r="644" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="644" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B644" s="7">
         <f>[1]B2_neuer_Gebietsstand!A639</f>
         <v>1</v>
       </c>
-      <c r="C644" s="27" t="s">
+      <c r="C644" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D644" s="27">
+      <c r="D644" s="17">
         <v>2008</v>
       </c>
-      <c r="E644" s="28">
+      <c r="E644" s="18">
         <v>20.6573595138854</v>
       </c>
-      <c r="F644" s="28">
+      <c r="F644" s="18">
         <v>11.153517802440618</v>
       </c>
     </row>
@@ -15929,21 +15929,21 @@
         <v>8.9651765868115589</v>
       </c>
     </row>
-    <row r="654" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="654" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B654" s="7">
         <f>[1]B2_neuer_Gebietsstand!A649</f>
         <v>2</v>
       </c>
-      <c r="C654" s="27" t="s">
+      <c r="C654" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="D654" s="27">
+      <c r="D654" s="17">
         <v>2008</v>
       </c>
-      <c r="E654" s="28">
+      <c r="E654" s="18">
         <v>25.495571095571094</v>
       </c>
-      <c r="F654" s="28">
+      <c r="F654" s="18">
         <v>14.204195804195804</v>
       </c>
     </row>
@@ -16145,21 +16145,21 @@
         <v>10.621982391366089</v>
       </c>
     </row>
-    <row r="666" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="666" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B666" s="7">
         <f>[1]B2_neuer_Gebietsstand!A661</f>
         <v>3</v>
       </c>
-      <c r="C666" s="27" t="s">
+      <c r="C666" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="D666" s="27">
+      <c r="D666" s="17">
         <v>2008</v>
       </c>
-      <c r="E666" s="28">
+      <c r="E666" s="18">
         <v>15.252127919639086</v>
       </c>
-      <c r="F666" s="28">
+      <c r="F666" s="18">
         <v>8.0072004800320027</v>
       </c>
     </row>
@@ -16469,39 +16469,39 @@
         <v>3.6485480268056589</v>
       </c>
     </row>
-    <row r="684" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="684" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B684" s="7">
         <f>[1]B2_neuer_Gebietsstand!A679</f>
         <v>4</v>
       </c>
-      <c r="C684" s="27" t="s">
+      <c r="C684" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="D684" s="27">
+      <c r="D684" s="17">
         <v>2008</v>
       </c>
-      <c r="E684" s="28">
+      <c r="E684" s="18">
         <v>20.154952785347614</v>
       </c>
-      <c r="F684" s="28">
+      <c r="F684" s="18">
         <v>10.346029532923506</v>
       </c>
     </row>
-    <row r="685" spans="2:6" s="26" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="685" spans="2:6" s="16" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B685" s="7">
         <f>[1]B2_neuer_Gebietsstand!A680</f>
         <v>0</v>
       </c>
-      <c r="C685" s="27" t="s">
+      <c r="C685" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="D685" s="27">
+      <c r="D685" s="17">
         <v>2008</v>
       </c>
-      <c r="E685" s="28">
+      <c r="E685" s="18">
         <v>20.580560020638604</v>
       </c>
-      <c r="F685" s="28">
+      <c r="F685" s="18">
         <v>11.009902561965431</v>
       </c>
     </row>

</xml_diff>